<commit_message>
PBL Modified Geolocation HU
</commit_message>
<xml_diff>
--- a/Historias de Ususario/PRODUCT_BARLOCK_ITEM.xlsx
+++ b/Historias de Ususario/PRODUCT_BARLOCK_ITEM.xlsx
@@ -251,9 +251,6 @@
     <t>Falta coger datos de Face y Google</t>
   </si>
   <si>
-    <t>FaltaActions en Api y cargar los datos</t>
-  </si>
-  <si>
     <t>Falta Implementar UI</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>Segunda Prioridad</t>
+  </si>
+  <si>
+    <t>cargar los datos</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1278,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1360,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1368,7 +1368,7 @@
         <v>0.85</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1383,10 +1383,10 @@
         <v>44306</v>
       </c>
       <c r="E6" s="9">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>0.6</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>0.15</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>0.15</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1549,13 +1549,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="10"/>
     </row>

</xml_diff>

<commit_message>
Update by Rolando's change
</commit_message>
<xml_diff>
--- a/Historias de Ususario/PRODUCT_BARLOCK_ITEM.xlsx
+++ b/Historias de Ususario/PRODUCT_BARLOCK_ITEM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="TASK" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
   <si>
     <t>Task</t>
   </si>
@@ -273,13 +273,28 @@
   </si>
   <si>
     <t>Generar xml de una camapaña</t>
+  </si>
+  <si>
+    <t>Implementar CRUD en el Backed de "Generar xml de una camapaña"</t>
+  </si>
+  <si>
+    <t>Integrar servicios del Backed y el FrontEnd para "Generar xml de una camapaña"</t>
+  </si>
+  <si>
+    <t>Crear interfaz para crear "Generar xml de una camapaña"</t>
+  </si>
+  <si>
+    <t>Dionis</t>
+  </si>
+  <si>
+    <t>Genear Apk y Acualizable de una campana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +314,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -366,6 +388,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,10 +671,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A3:G44"/>
+  <dimension ref="A3:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,6 +1283,57 @@
     <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="14">
+        <v>44306</v>
+      </c>
+      <c r="F45" s="14">
+        <v>44314</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="14">
+        <v>44306</v>
+      </c>
+      <c r="F46" s="14">
+        <v>44314</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="14">
+        <v>44306</v>
+      </c>
+      <c r="F47" s="14">
+        <v>44314</v>
       </c>
     </row>
   </sheetData>
@@ -1280,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,10 +1552,18 @@
       <c r="B11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="14">
+        <v>44306</v>
+      </c>
+      <c r="D11" s="14">
+        <v>44314</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>

</xml_diff>

<commit_message>
Campaign List Ordered whith Search ProductBackLog Updated
</commit_message>
<xml_diff>
--- a/Historias de Ususario/PRODUCT_BARLOCK_ITEM.xlsx
+++ b/Historias de Ususario/PRODUCT_BARLOCK_ITEM.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TASK" sheetId="1" r:id="rId1"/>
@@ -260,9 +260,6 @@
     <t>Listar Campañas</t>
   </si>
   <si>
-    <t>Falta Implementar Busqueda y Ordenamiento por Columnas.</t>
-  </si>
-  <si>
     <t>Falta Actions en Api, Crear Servicio y finalizar la UI.</t>
   </si>
   <si>
@@ -288,12 +285,15 @@
   </si>
   <si>
     <t>Genear Apk y Acualizable de una campana</t>
+  </si>
+  <si>
+    <t>Falta Vizualizar los Logos de la Campaña. Y Revisar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -673,19 +673,19 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A3:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+    <sheetView topLeftCell="B8" workbookViewId="0">
       <selection activeCell="C45" sqref="C45:C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="99" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -708,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -725,7 +725,7 @@
         <v>44278</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -742,7 +742,7 @@
         <v>44278</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -759,7 +759,7 @@
         <v>44278</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -776,7 +776,7 @@
         <v>44278</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>40</v>
       </c>
@@ -796,7 +796,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -810,7 +810,7 @@
         <v>44278</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -824,7 +824,7 @@
         <v>44290</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -841,7 +841,7 @@
         <v>44290</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -861,7 +861,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -879,7 +879,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -896,7 +896,7 @@
         <v>44295</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -913,7 +913,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -930,7 +930,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="17" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -947,7 +947,7 @@
         <v>44283</v>
       </c>
     </row>
-    <row r="18" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -964,7 +964,7 @@
         <v>44283</v>
       </c>
     </row>
-    <row r="19" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -981,7 +981,7 @@
         <v>44280</v>
       </c>
     </row>
-    <row r="20" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
@@ -998,7 +998,7 @@
         <v>44283</v>
       </c>
     </row>
-    <row r="21" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>44284</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>29</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>19</v>
       </c>
@@ -1080,7 +1080,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -1106,7 +1106,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>20</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>23</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>37</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>28</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>32</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>33</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>34</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>51</v>
       </c>
@@ -1246,7 +1246,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>38</v>
       </c>
@@ -1270,30 +1270,30 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
         <v>86</v>
-      </c>
-      <c r="D45" t="s">
-        <v>87</v>
       </c>
       <c r="E45" s="14">
         <v>44306</v>
@@ -1302,15 +1302,15 @@
         <v>44314</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" t="s">
         <v>86</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
       </c>
       <c r="E46" s="14">
         <v>44306</v>
@@ -1319,15 +1319,15 @@
         <v>44314</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="D47" t="s">
         <v>86</v>
-      </c>
-      <c r="D47" t="s">
-        <v>87</v>
       </c>
       <c r="E47" s="14">
         <v>44306</v>
@@ -1355,19 +1355,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="76" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>62</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>62</v>
       </c>
@@ -1443,13 +1443,13 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="9">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>62</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>62</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>62</v>
       </c>
@@ -1504,10 +1504,10 @@
         <v>0.15</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>62</v>
       </c>
@@ -1524,10 +1524,10 @@
         <v>0.15</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>62</v>
       </c>
@@ -1545,12 +1545,12 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="14">
         <v>44306</v>
@@ -1562,10 +1562,10 @@
         <v>0.2</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1573,7 +1573,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1581,7 +1581,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1589,7 +1589,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1597,7 +1597,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1605,7 +1605,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1613,7 +1613,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1621,7 +1621,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1629,7 +1629,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1637,15 +1637,15 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>80</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>81</v>
       </c>
       <c r="B23" s="10"/>
     </row>
@@ -1660,10 +1660,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>